<commit_message>
restructuring and populating initial generation of GA
</commit_message>
<xml_diff>
--- a/data/sample.xlsx
+++ b/data/sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeeGoG\PycharmProjects\ReleasePlanningLP\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeeGoG\PycharmProjects\MobileReleasePlanner\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="54">
   <si>
     <t>Feature f(i)</t>
   </si>
@@ -141,6 +141,51 @@
   </si>
   <si>
     <t>Feature Key</t>
+  </si>
+  <si>
+    <t>F7</t>
+  </si>
+  <si>
+    <t>F6</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F8</t>
+  </si>
+  <si>
+    <t>F9</t>
+  </si>
+  <si>
+    <t>F10</t>
+  </si>
+  <si>
+    <t>F11</t>
+  </si>
+  <si>
+    <t>F12</t>
+  </si>
+  <si>
+    <t>F13</t>
+  </si>
+  <si>
+    <t>F14</t>
+  </si>
+  <si>
+    <t>F15</t>
   </si>
 </sst>
 </file>
@@ -477,7 +522,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -525,8 +570,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>1</v>
+      <c r="A3" t="s">
+        <v>45</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
@@ -548,8 +593,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>2</v>
+      <c r="A4" t="s">
+        <v>44</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
@@ -571,8 +616,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>3</v>
+      <c r="A5" t="s">
+        <v>43</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
@@ -594,8 +639,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>4</v>
+      <c r="A6" t="s">
+        <v>42</v>
       </c>
       <c r="B6" t="s">
         <v>26</v>
@@ -617,8 +662,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>5</v>
+      <c r="A7" t="s">
+        <v>41</v>
       </c>
       <c r="B7" t="s">
         <v>27</v>
@@ -640,8 +685,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>6</v>
+      <c r="A8" t="s">
+        <v>40</v>
       </c>
       <c r="B8" t="s">
         <v>28</v>
@@ -663,8 +708,8 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>7</v>
+      <c r="A9" t="s">
+        <v>39</v>
       </c>
       <c r="B9" t="s">
         <v>29</v>
@@ -686,8 +731,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>8</v>
+      <c r="A10" t="s">
+        <v>46</v>
       </c>
       <c r="B10" t="s">
         <v>30</v>
@@ -709,8 +754,8 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>9</v>
+      <c r="A11" t="s">
+        <v>47</v>
       </c>
       <c r="B11" t="s">
         <v>31</v>
@@ -732,8 +777,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>10</v>
+      <c r="A12" t="s">
+        <v>48</v>
       </c>
       <c r="B12" t="s">
         <v>32</v>
@@ -755,8 +800,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>11</v>
+      <c r="A13" t="s">
+        <v>49</v>
       </c>
       <c r="B13" t="s">
         <v>33</v>
@@ -778,8 +823,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>12</v>
+      <c r="A14" t="s">
+        <v>50</v>
       </c>
       <c r="B14" t="s">
         <v>34</v>
@@ -801,8 +846,8 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>13</v>
+      <c r="A15" t="s">
+        <v>51</v>
       </c>
       <c r="B15" t="s">
         <v>35</v>
@@ -824,8 +869,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>14</v>
+      <c r="A16" t="s">
+        <v>52</v>
       </c>
       <c r="B16" t="s">
         <v>36</v>
@@ -847,8 +892,8 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>15</v>
+      <c r="A17" t="s">
+        <v>53</v>
       </c>
       <c r="B17" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
prepared features for mobile planning
</commit_message>
<xml_diff>
--- a/data/sample.xlsx
+++ b/data/sample.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
   <si>
     <t>Feature f(i)</t>
   </si>
@@ -50,12 +50,6 @@
     <t>(0, 0, 9)</t>
   </si>
   <si>
-    <t>Stakeholder S (1)</t>
-  </si>
-  <si>
-    <t>Stakeholder S (2)</t>
-  </si>
-  <si>
     <t>(0, 3, 6)</t>
   </si>
   <si>
@@ -80,18 +74,6 @@
     <t>Number of releases (R)</t>
   </si>
   <si>
-    <t>Urgency u(2,i)</t>
-  </si>
-  <si>
-    <t>Value v(2,i)</t>
-  </si>
-  <si>
-    <t>Urgency u(1,i)</t>
-  </si>
-  <si>
-    <t>Value v(1,i)</t>
-  </si>
-  <si>
     <t>Total effort estimation</t>
   </si>
   <si>
@@ -186,6 +168,18 @@
   </si>
   <si>
     <t>F15</t>
+  </si>
+  <si>
+    <t>Stakeholder S (1), Value v(1,i)</t>
+  </si>
+  <si>
+    <t>Stakeholder S (1), Urgency u(1,i)</t>
+  </si>
+  <si>
+    <t>Stakeholder S (2), Value v(2,i)</t>
+  </si>
+  <si>
+    <t>Stakeholder S (2), Urgency u(2,i)</t>
   </si>
 </sst>
 </file>
@@ -229,16 +223,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -535,407 +525,392 @@
     <col min="7" max="7" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C1" s="3"/>
-      <c r="D1" s="4" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
         <v>8</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
         <v>4</v>
-      </c>
-      <c r="D4">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F6">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D8">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F8">
         <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C9">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G10" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C11">
+        <v>0.5</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
         <v>1</v>
       </c>
-      <c r="D11">
-        <v>6</v>
-      </c>
-      <c r="E11" t="s">
-        <v>3</v>
-      </c>
       <c r="F11">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C12">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G12" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F13">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E14" t="s">
         <v>3</v>
       </c>
       <c r="F14">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G14" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
         <v>8</v>
       </c>
-      <c r="D15">
-        <v>7</v>
-      </c>
       <c r="E15" t="s">
         <v>3</v>
       </c>
       <c r="F15">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G15" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D16">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F16">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>53</v>
-      </c>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="C17">
-        <v>5</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17">
-        <v>5</v>
-      </c>
-      <c r="G17" t="s">
+        <f>SUM(C2:C16)</f>
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18">
-        <f>SUM(C3:C17)</f>
-        <v>52.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="2">
+      <c r="C18" s="2">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>